<commit_message>
don't read whole sheet at start
</commit_message>
<xml_diff>
--- a/samples/squared.xlsx
+++ b/samples/squared.xlsx
@@ -491,7 +491,7 @@
   <dimension ref="C4:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -524,11 +524,11 @@
     </row>
     <row r="7" spans="3:4">
       <c r="C7">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="3:4">

</xml_diff>